<commit_message>
jupyter notebook + excel bug fix
</commit_message>
<xml_diff>
--- a/Models/Industry_model/Input/Glass/Data/parameters.xlsx
+++ b/Models/Industry_model/Input/Glass/Data/parameters.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin.girard/Documents/Code/Etude/Energy-Alternatives-Planing/Models/Industry_model/Input/Steel/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engie-my.sharepoint.com/personal/kv6345_engie_com/Documents/Documents/5-Python/Energy-Alternatives-Planing/Models/Industry_model/Input/Glass/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8DE5E9-6BF6-404C-999D-2D9071F17AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{69860596-7255-4AC2-A731-2E5CCEF0ECEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="2580" windowWidth="23740" windowHeight="11760" activeTab="1" xr2:uid="{72F20DD2-FD61-154B-B48D-F6B531A3694C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{72F20DD2-FD61-154B-B48D-F6B531A3694C}"/>
   </bookViews>
   <sheets>
     <sheet name="TECHNOLOGIES" sheetId="1" r:id="rId1"/>
     <sheet name="RESOURCES" sheetId="2" r:id="rId2"/>
     <sheet name="TECHNOLOGIES_RESOURCES" sheetId="3" r:id="rId3"/>
+    <sheet name="SOURCES" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -34,8 +37,65 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={307A3C29-139E-44FE-82D5-E0C1D898C9C8}</author>
+    <author>tc={0281061E-3C99-4E77-B0D5-C23E357B022E}</author>
+  </authors>
+  <commentList>
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{307A3C29-139E-44FE-82D5-E0C1D898C9C8}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    https://www.researchgate.net/publication/265491948_End-of-Waste_Criteria_for_Glass_Cullet_Technical_Proposals</t>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="1" shapeId="0" xr:uid="{0281061E-3C99-4E77-B0D5-C23E357B022E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    8%boost...</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
+  <si>
+    <t>TECHNOLOGIES</t>
+  </si>
+  <si>
+    <t>emissions_t</t>
+  </si>
+  <si>
+    <t>capex</t>
+  </si>
+  <si>
+    <t>lifetime</t>
+  </si>
+  <si>
+    <t>discount_rate</t>
+  </si>
+  <si>
+    <t>CRF</t>
+  </si>
+  <si>
+    <t>flow_cost_t</t>
+  </si>
+  <si>
+    <t>forced_prod_ratio</t>
+  </si>
+  <si>
+    <t>max_capacity_t</t>
+  </si>
+  <si>
+    <t>forced_resource</t>
+  </si>
   <si>
     <t>Scrap</t>
   </si>
@@ -46,6 +106,9 @@
     <t>BF-BOF</t>
   </si>
   <si>
+    <t>Steel</t>
+  </si>
+  <si>
     <t>H2-BF-BOF</t>
   </si>
   <si>
@@ -70,103 +133,94 @@
     <t>CCS</t>
   </si>
   <si>
-    <t>TECHNOLOGIES</t>
+    <t>E_boiler</t>
+  </si>
+  <si>
+    <t>Gas_boiler</t>
+  </si>
+  <si>
+    <t>SMR</t>
+  </si>
+  <si>
+    <t>Electrolyser</t>
+  </si>
+  <si>
+    <t>Methanisation</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>RESOURCES</t>
+  </si>
+  <si>
+    <t>emissions_r</t>
+  </si>
+  <si>
+    <t>flow_cost_r</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>max_volume</t>
+  </si>
+  <si>
+    <t>production_error_margin</t>
+  </si>
+  <si>
+    <t>Coal</t>
+  </si>
+  <si>
+    <t>Biomass</t>
+  </si>
+  <si>
+    <t>Oil</t>
+  </si>
+  <si>
+    <t>Electricity</t>
   </si>
   <si>
     <t>CO2</t>
   </si>
   <si>
-    <t>capex</t>
-  </si>
-  <si>
-    <t>lifetime</t>
-  </si>
-  <si>
-    <t>discount_rate</t>
-  </si>
-  <si>
-    <t>CRF</t>
-  </si>
-  <si>
-    <t>Coal</t>
-  </si>
-  <si>
-    <t>Biomass</t>
-  </si>
-  <si>
-    <t>Oil</t>
-  </si>
-  <si>
-    <t>Electricity</t>
-  </si>
-  <si>
-    <t>Gas</t>
-  </si>
-  <si>
-    <t>E_boiler</t>
-  </si>
-  <si>
-    <t>Gas_boiler</t>
-  </si>
-  <si>
-    <t>SMR</t>
-  </si>
-  <si>
-    <t>Electrolyser</t>
+    <t>Hydrogen</t>
+  </si>
+  <si>
+    <t>Steam</t>
   </si>
   <si>
     <t>Water</t>
   </si>
   <si>
-    <t>Steel</t>
-  </si>
-  <si>
     <t>ore_pellet</t>
   </si>
   <si>
     <t>scrap_steel</t>
   </si>
   <si>
-    <t>Hydrogen</t>
-  </si>
-  <si>
-    <t>Steam</t>
-  </si>
-  <si>
-    <t>output</t>
-  </si>
-  <si>
-    <t>Methanisation</t>
-  </si>
-  <si>
-    <t>flow_cost_r</t>
-  </si>
-  <si>
-    <t>flow_cost_t</t>
-  </si>
-  <si>
-    <t>emissions_t</t>
-  </si>
-  <si>
-    <t>emissions_r</t>
-  </si>
-  <si>
-    <t>forced_prod_ratio</t>
-  </si>
-  <si>
-    <t>max_capacity_t</t>
-  </si>
-  <si>
-    <t>production_error_margin</t>
-  </si>
-  <si>
-    <t>max_volume</t>
-  </si>
-  <si>
-    <t>forced_resource</t>
-  </si>
-  <si>
-    <t>RESOURCES</t>
+    <t>Gas furnace</t>
+  </si>
+  <si>
+    <t>Electric furnace</t>
+  </si>
+  <si>
+    <t>Cullet</t>
+  </si>
+  <si>
+    <t>Gas furnace + E-boost</t>
+  </si>
+  <si>
+    <t>Cullet price</t>
+  </si>
+  <si>
+    <t>(PDF) End-of-Waste Criteria for Glass Cullet: Technical Proposals (researchgate.net)</t>
+  </si>
+  <si>
+    <t>TECHNOLOGIES CAPEX</t>
+  </si>
+  <si>
+    <t>Decarbonisation options for the Dutch container and tableware glass industry (pbl.nl)</t>
   </si>
 </sst>
 </file>
@@ -176,7 +230,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -192,8 +246,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -248,8 +316,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -299,24 +373,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="9"/>
-      </right>
-      <top style="thin">
-        <color theme="9"/>
-      </top>
-      <bottom style="thin">
-        <color theme="9"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -334,14 +396,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -357,8 +421,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="ROGEAU Antoine (ENGIE Impact)" id="{161872B8-199F-4E3C-8A5F-613E30FB2168}" userId="S::KV6345@engie.com::2fc49cd1-1025-4c77-95fe-1e365f355d2a" providerId="AD"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -652,90 +722,105 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="G2" dT="2022-08-10T09:42:45.06" personId="{161872B8-199F-4E3C-8A5F-613E30FB2168}" id="{307A3C29-139E-44FE-82D5-E0C1D898C9C8}">
+    <text>https://www.researchgate.net/publication/265491948_End-of-Waste_Criteria_for_Glass_Cullet_Technical_Proposals</text>
+  </threadedComment>
+  <threadedComment ref="A6" dT="2022-08-10T10:38:30.29" personId="{161872B8-199F-4E3C-8A5F-613E30FB2168}" id="{0281061E-3C99-4E77-B0D5-C23E357B022E}">
+    <text>8%boost...</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CEC0513-801E-2542-89D6-117D6191FB3E}">
-  <dimension ref="A1:J17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CEC0513-801E-2542-89D6-117D6191FB3E}">
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="1" max="1" width="15.125" customWidth="1"/>
     <col min="8" max="8" width="19.5" customWidth="1"/>
     <col min="10" max="10" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="G2">
-        <v>180</v>
+        <v>45</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="9"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
+        <v>11</v>
+      </c>
+      <c r="B3" s="23">
         <v>0.26</v>
       </c>
-      <c r="G3">
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23">
         <v>114</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
       <c r="J3" s="9"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="B4">
-        <v>1.766</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="C4">
         <v>218.3</v>
       </c>
       <c r="D4">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E4">
         <v>0.1</v>
@@ -751,21 +836,21 @@
       </c>
       <c r="I4" s="7"/>
       <c r="J4" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="B5">
-        <v>1.5300499999999999</v>
+        <v>3.9E-2</v>
       </c>
       <c r="C5">
-        <v>218.3</v>
+        <v>0.5</v>
       </c>
       <c r="D5">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E5">
         <v>0.1</v>
@@ -778,18 +863,18 @@
       </c>
       <c r="I5" s="16"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="B6">
-        <v>1.766</v>
+        <v>0.26</v>
       </c>
       <c r="C6">
         <v>218.3</v>
       </c>
       <c r="D6">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E6">
         <v>0.1</v>
@@ -801,209 +886,43 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <v>184</v>
-      </c>
-      <c r="D7">
-        <v>20</v>
-      </c>
-      <c r="E7">
-        <v>0.1</v>
-      </c>
-      <c r="F7">
-        <v>0.11745962477254576</v>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>-1</v>
       </c>
       <c r="G7">
-        <v>53.2</v>
-      </c>
-      <c r="H7" s="16">
-        <v>0.34</v>
-      </c>
-      <c r="J7" s="17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8">
-        <v>414</v>
-      </c>
-      <c r="D8">
-        <v>20</v>
-      </c>
-      <c r="E8">
-        <v>0.1</v>
-      </c>
-      <c r="F8">
-        <v>0.11745962477254576</v>
-      </c>
-      <c r="G8">
-        <v>53.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>0.82899999999999996</v>
-      </c>
-      <c r="C9">
-        <v>414</v>
-      </c>
-      <c r="D9">
-        <v>20</v>
-      </c>
-      <c r="E9">
-        <v>0.1</v>
-      </c>
-      <c r="F9">
-        <v>0.11745962477254576</v>
-      </c>
-      <c r="G9">
-        <v>53.2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>1.355</v>
-      </c>
-      <c r="C10">
-        <v>414</v>
-      </c>
-      <c r="D10">
-        <v>20</v>
-      </c>
-      <c r="E10">
-        <v>0.1</v>
-      </c>
-      <c r="F10">
-        <v>0.11745962477254576</v>
-      </c>
-      <c r="G10">
-        <v>53.2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>1.355</v>
-      </c>
-      <c r="C11">
-        <v>414</v>
-      </c>
-      <c r="D11">
-        <v>20</v>
-      </c>
-      <c r="E11">
-        <v>0.1</v>
-      </c>
-      <c r="F11">
-        <v>0.11745962477254576</v>
-      </c>
-      <c r="G11">
-        <v>53.2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>-1</v>
-      </c>
-      <c r="G12">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15">
-        <v>12.13</v>
-      </c>
-      <c r="C15">
-        <v>3448.3536819299948</v>
-      </c>
-      <c r="D15">
-        <v>25</v>
-      </c>
-      <c r="E15">
-        <v>0.1</v>
-      </c>
-      <c r="F15">
-        <v>0.11016807219002084</v>
-      </c>
-      <c r="G15">
-        <v>324.97573965832413</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>10</v>
-      </c>
-      <c r="E16">
-        <v>0.1</v>
-      </c>
-      <c r="F16">
-        <v>0.16274539488251155</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="10">
         <f>0.000001*-84*14500</f>
         <v>-1.218</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="G17" s="4">
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
         <f>49.2578*13</f>
         <v>640.35140000000001</v>
       </c>
-      <c r="I17">
+      <c r="I8">
         <v>860000</v>
       </c>
-      <c r="J17" t="s">
-        <v>21</v>
+      <c r="J8" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1011,35 +930,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7586E3A9-C0EE-6F42-8EFF-5D7691C2A1FF}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="B2" s="10">
         <f>29308*0.00001621</f>
@@ -1053,9 +972,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="B3" s="10">
         <f>0.000001*9*16900</f>
@@ -1068,9 +987,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B4" s="10">
         <f>41816*0.0000136</f>
@@ -1084,9 +1003,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="B5" s="10">
         <v>0.06</v>
@@ -1098,9 +1017,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B6" s="10">
         <f>45998*0.0000097</f>
@@ -1110,9 +1029,9 @@
         <v>291.66900000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="B7" s="4">
         <v>-1</v>
@@ -1124,9 +1043,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B8" s="15">
         <v>0</v>
@@ -1138,9 +1057,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B9" s="15">
         <v>0</v>
@@ -1152,9 +1071,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="B10" s="14">
         <v>0</v>
@@ -1166,9 +1085,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1180,9 +1099,9 @@
         <v>15000000</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1194,9 +1113,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -1210,6 +1129,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1218,65 +1138,65 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+    <col min="1" max="1" width="14.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
         <v>21</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="L1" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="M1" s="22" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
-        <v>10</v>
       </c>
       <c r="G2" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
         <v>22</v>
       </c>
       <c r="E3">
@@ -1286,8 +1206,8 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="20" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
         <v>23</v>
       </c>
       <c r="F4">
@@ -1297,8 +1217,8 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
         <v>24</v>
       </c>
       <c r="F5" s="4">
@@ -1308,26 +1228,26 @@
         <v>4.45</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="20" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
         <v>25</v>
       </c>
       <c r="H6" s="4">
         <v>55</v>
       </c>
-      <c r="I6" s="18"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="21" t="s">
-        <v>33</v>
+      <c r="I6" s="17"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>26</v>
       </c>
       <c r="F7">
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E8" s="4">
         <f>0.004</f>
@@ -1340,9 +1260,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E9">
         <v>0.14000000000000001</v>
@@ -1354,9 +1274,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>0.53336811799229455</v>
@@ -1374,9 +1294,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>0.45336290029345033</v>
@@ -1397,9 +1317,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>0.24762981812463489</v>
@@ -1420,9 +1340,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E13">
         <v>0.88000000000000012</v>
@@ -1438,9 +1358,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E14">
         <v>1.26</v>
@@ -1458,9 +1378,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E15">
         <v>1.26</v>
@@ -1475,9 +1395,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C16">
         <v>0.19192346461228307</v>
@@ -1495,9 +1415,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>0.12848432777391336</v>
@@ -1517,5 +1437,42 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D138BF4-DEBD-48F7-A4E3-83C7907FE87D}">
+  <dimension ref="A2:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="https://www.researchgate.net/publication/265491948_End-of-Waste_Criteria_for_Glass_Cullet_Technical_Proposals" xr:uid="{078984C0-84A6-473B-88B2-CD1EA9A51DDE}"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://www.pbl.nl/sites/default/files/downloads/pbl-2019-decarbonisation-options-for-the-dutch-container_and_tableware_glass_industry_3720.pdf" xr:uid="{29E0DD23-6F29-49F7-8F80-8B6D9AD9147F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>